<commit_message>
- Se actualizan documentos - Se actualizan implementaciones de List según el laboratorio de ordenamientos-1
</commit_message>
<xml_diff>
--- a/Docs/ISIS1225 - Tablas de Datos Lab 4.xlsx
+++ b/Docs/ISIS1225 - Tablas de Datos Lab 4.xlsx
@@ -117,7 +117,6 @@
     <font>
       <b/>
       <sz val="11.000000"/>
-      <color indexed="64"/>
       <name val="Dax-Regular"/>
     </font>
     <font>
@@ -249,7 +248,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11.000000"/>
-        <color indexed="64"/>
         <name val="Dax-Regular"/>
         <scheme val="none"/>
       </font>
@@ -263,7 +261,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11.000000"/>
-        <color indexed="64"/>
         <name val="Dax-Regular"/>
         <scheme val="none"/>
       </font>
@@ -277,7 +274,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11.000000"/>
-        <color indexed="64"/>
         <name val="Dax-Regular"/>
         <scheme val="none"/>
       </font>
@@ -295,7 +291,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11.000000"/>
-        <color indexed="64"/>
         <name val="Dax-Regular"/>
         <scheme val="none"/>
       </font>
@@ -315,7 +310,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11.000000"/>
-        <color indexed="64"/>
         <name val="Dax-Regular"/>
         <scheme val="none"/>
       </font>
@@ -335,7 +329,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11.000000"/>
-        <color indexed="64"/>
         <name val="Dax-Regular"/>
         <scheme val="none"/>
       </font>
@@ -397,7 +390,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11.000000"/>
-        <color indexed="64"/>
         <name val="Dax-Regular"/>
         <scheme val="none"/>
       </font>
@@ -411,7 +403,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11.000000"/>
-        <color indexed="64"/>
         <name val="Dax-Regular"/>
         <scheme val="none"/>
       </font>
@@ -425,7 +416,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11.000000"/>
-        <color indexed="64"/>
         <name val="Dax-Regular"/>
         <scheme val="none"/>
       </font>
@@ -443,7 +433,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11.000000"/>
-        <color indexed="64"/>
         <name val="Dax-Regular"/>
         <scheme val="none"/>
       </font>
@@ -463,7 +452,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11.000000"/>
-        <color indexed="64"/>
         <name val="Dax-Regular"/>
         <scheme val="none"/>
       </font>
@@ -483,7 +471,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11.000000"/>
-        <color indexed="64"/>
         <name val="Dax-Regular"/>
         <scheme val="none"/>
       </font>
@@ -547,7 +534,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" b="1"/>
-              <a:t> Queue</a:t>
+              <a:t> Enqueue</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" b="1"/>
           </a:p>
@@ -1272,7 +1259,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" b="1"/>
-              <a:t>Comparación de tiempos de ejecucion para Queue</a:t>
+              <a:t>Comparación de tiempos de ejecucion para Dequeue</a:t>
             </a:r>
             <a:endParaRPr/>
           </a:p>
@@ -1997,7 +1984,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" b="1"/>
-              <a:t>Comparación de tiempos de ejecucion para Queue</a:t>
+              <a:t>Comparación de tiempos de ejecucion para Peek</a:t>
             </a:r>
             <a:endParaRPr/>
           </a:p>
@@ -2726,7 +2713,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" b="1"/>
-              <a:t> Stack</a:t>
+              <a:t> Push</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" b="1"/>
           </a:p>
@@ -3455,7 +3442,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" b="1"/>
-              <a:t> Stack</a:t>
+              <a:t> Pop</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" b="1"/>
           </a:p>
@@ -4184,7 +4171,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" b="1"/>
-              <a:t> Stack</a:t>
+              <a:t> Top</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" b="1"/>
           </a:p>

</xml_diff>